<commit_message>
Updating CPRA post-proc scripts to include MS River stations. Changing NOV-14 observation data from USACE to USGS.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Datum_Conversion.xlsx
+++ b/output/cpra_postproc/Datum_Conversion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Desktop\CPRA_Post_Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Desktop\working\Barry_CPRA_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
   <si>
     <t>USACE</t>
   </si>
@@ -60,6 +60,30 @@
   </si>
   <si>
     <t>08017118</t>
+  </si>
+  <si>
+    <t>01400</t>
+  </si>
+  <si>
+    <t>01390</t>
+  </si>
+  <si>
+    <t>01300</t>
+  </si>
+  <si>
+    <t>01280</t>
+  </si>
+  <si>
+    <t>01275</t>
+  </si>
+  <si>
+    <t>01260</t>
+  </si>
+  <si>
+    <t>03780</t>
+  </si>
+  <si>
+    <t>291929089562600</t>
   </si>
 </sst>
 </file>
@@ -379,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,10 +534,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -627,6 +651,83 @@
       </c>
       <c r="C22" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1">
+        <v>-0.82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-0.76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-1.1100000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusitng NOV13/14 observation locations.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Datum_Conversion.xlsx
+++ b/output/cpra_postproc/Datum_Conversion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Desktop\working\Barry_CPRA_Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Desktop\cpra_hydrograph_plotter\cpra_hydrograph_plotter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -83,7 +83,7 @@
     <t>03780</t>
   </si>
   <si>
-    <t>291929089562600</t>
+    <t>07380260</t>
   </si>
 </sst>
 </file>
@@ -406,12 +406,15 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="15.734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -433,7 +436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -444,7 +447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -455,7 +458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -466,7 +469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -477,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -488,7 +491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -499,7 +502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -510,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -521,29 +524,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -554,7 +557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -565,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -576,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -587,7 +590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -598,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -609,7 +612,7 @@
         <v>-0.35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -620,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -631,7 +634,7 @@
         <v>-6.31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -642,7 +645,7 @@
         <v>-2.25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -653,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -664,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -675,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -686,7 +689,7 @@
         <v>-0.82</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -697,7 +700,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -708,7 +711,7 @@
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -719,7 +722,7 @@
         <v>-0.76</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updating to the latest CPRA slide deck workflow.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Datum_Conversion.xlsx
+++ b/output/cpra_postproc/Datum_Conversion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Desktop\cpra_hydrograph_plotter\cpra_hydrograph_plotter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Documents\PROJECTS\CPRA\2020_Season\AL032020\NAM\2020060406\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>USACE</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>07380260</t>
+  </si>
+  <si>
+    <t>073802332</t>
+  </si>
+  <si>
+    <t>82740</t>
+  </si>
+  <si>
+    <t>76305</t>
   </si>
 </sst>
 </file>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -427,10 +436,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>76065</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -484,11 +493,11 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2">
-        <v>82742</v>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -532,7 +541,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -661,10 +670,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -672,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -683,10 +692,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1">
-        <v>-0.82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -694,10 +703,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1">
-        <v>-0.7</v>
+        <v>-0.82</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -705,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1">
-        <v>-0.55000000000000004</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -716,10 +725,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="1">
-        <v>-0.76</v>
+        <v>-0.55000000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -727,9 +736,20 @@
         <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-0.76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <v>-1.1100000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating CPRA slide decks to include additional stations.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Datum_Conversion.xlsx
+++ b/output/cpra_postproc/Datum_Conversion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Documents\PROJECTS\CPRA\2020_Season\AL032020\NAM\2020060406\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Documents\PROJECTS\CPRA\2020_Season\AL032020\NAM\2020060518\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>USACE</t>
   </si>
@@ -89,10 +89,16 @@
     <t>073802332</t>
   </si>
   <si>
-    <t>82740</t>
-  </si>
-  <si>
     <t>76305</t>
+  </si>
+  <si>
+    <t>01480</t>
+  </si>
+  <si>
+    <t>073814675</t>
+  </si>
+  <si>
+    <t>82742</t>
   </si>
 </sst>
 </file>
@@ -412,18 +418,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -445,7 +451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -456,7 +462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -467,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -478,7 +484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -489,18 +495,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1">
-        <v>-0.16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -511,7 +517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -522,7 +528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -533,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -544,7 +550,7 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -555,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -566,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -577,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -588,7 +594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -599,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -610,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -621,7 +627,7 @@
         <v>-0.35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -632,7 +638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -643,7 +649,7 @@
         <v>-6.31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -654,7 +660,7 @@
         <v>-2.25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -665,18 +671,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
         <v>-0.08</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -687,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -698,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -709,7 +715,7 @@
         <v>-0.82</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -720,7 +726,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -731,7 +737,7 @@
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -742,7 +748,7 @@
         <v>-0.76</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -751,6 +757,39 @@
       </c>
       <c r="C30" s="1">
         <v>-1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>76560</v>
+      </c>
+      <c r="C32" s="1">
+        <v>-1.214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating CPRA slide deck generation tools. Re-order of slide deck; change in text; additional triggers.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Datum_Conversion.xlsx
+++ b/output/cpra_postproc/Datum_Conversion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Documents\PROJECTS\CPRA\2020_Season\AL032020\NAM\2020060518\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Documents\PROJECTS\CPRA\2020_Season\SlideDeckUpdates_07012020\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>USACE</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>82875</t>
-  </si>
-  <si>
-    <t>76220</t>
   </si>
   <si>
     <t>76230</t>
@@ -418,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +442,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -488,8 +485,8 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2">
-        <v>82770</v>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -499,8 +496,8 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
+      <c r="B7" s="2">
+        <v>85760</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -511,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="2">
-        <v>85760</v>
+        <v>76010</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -522,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="2">
-        <v>76010</v>
+        <v>82715</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -530,24 +527,24 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2">
-        <v>82715</v>
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>-4.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -566,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -577,7 +574,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -588,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -599,18 +596,18 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>8</v>
+      <c r="B17" s="2">
+        <v>76025</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -618,21 +615,21 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="1">
-        <v>-0.35</v>
+        <v>-6.31</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2">
-        <v>76025</v>
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -640,32 +637,32 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1">
-        <v>-6.31</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="2">
-        <v>76593</v>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C21" s="1">
-        <v>-2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -676,10 +673,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1">
-        <v>-0.08</v>
+        <v>-0.82</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -687,10 +684,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,10 +695,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>-0.55000000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,10 +706,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1">
-        <v>-0.82</v>
+        <v>-0.76</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1">
-        <v>-0.7</v>
+        <v>-1.1100000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -731,64 +728,31 @@
         <v>0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C28" s="1">
-        <v>-0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>17</v>
+      <c r="B29" s="2">
+        <v>76560</v>
       </c>
       <c r="C29" s="1">
-        <v>-0.76</v>
+        <v>-1.214</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1">
-        <v>-1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="2">
-        <v>76560</v>
-      </c>
-      <c r="C32" s="1">
-        <v>-1.214</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>